<commit_message>
forgot to push this commit
</commit_message>
<xml_diff>
--- a/time_findSameHands_Tomas.xlsx
+++ b/time_findSameHands_Tomas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rytis\Documents\MyDocuments\MyApps\findSameHands_Tomas_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D816308-A8B6-4E20-BF2D-654BB8FEDE48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA798E7-4C73-49DE-8B1C-CC5EB751D900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>check on GitHub</t>
+  </si>
+  <si>
+    <t>2020 09 24</t>
+  </si>
+  <si>
+    <t>fixing problem. String to put in the file reaches memory limit</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -667,38 +673,44 @@
         <v>0.15972222222222235</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>2020 09 11</v>
-      </c>
-      <c r="B6" s="10">
-        <f t="shared" si="2"/>
-        <v>0.75694444444444453</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="13">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25">
         <f t="shared" si="0"/>
-        <v>-0.75694444444444453</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>0.10069444444444442</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28">
+        <f>SUM(E6)</f>
+        <v>0.10069444444444442</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B7" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.93402777777777779</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.93402777777777779</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -706,7 +718,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B8" s="10">
         <f t="shared" si="2"/>
@@ -724,7 +736,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B9" s="10">
         <f t="shared" si="2"/>
@@ -742,7 +754,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B10" s="10">
         <f t="shared" si="2"/>
@@ -760,7 +772,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B11" s="10">
         <f t="shared" si="2"/>
@@ -778,7 +790,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B12" s="10">
         <f t="shared" si="2"/>
@@ -796,7 +808,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B13" s="10">
         <f t="shared" si="2"/>
@@ -814,7 +826,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="str">
         <f>A13</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B14" s="11">
         <f t="shared" si="2"/>
@@ -832,7 +844,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B15" s="10">
         <f t="shared" si="2"/>
@@ -850,7 +862,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B16" s="10">
         <f t="shared" si="2"/>
@@ -868,7 +880,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B17" s="10">
         <f t="shared" si="2"/>
@@ -886,7 +898,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B18" s="10">
         <f t="shared" si="2"/>
@@ -904,7 +916,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B19" s="10">
         <f t="shared" si="2"/>
@@ -922,7 +934,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B20" s="10">
         <f t="shared" si="2"/>
@@ -940,7 +952,7 @@
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B21" s="10">
         <f t="shared" si="2"/>
@@ -958,7 +970,7 @@
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B22" s="10">
         <f t="shared" si="2"/>
@@ -976,7 +988,7 @@
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B23" s="10">
         <f t="shared" si="2"/>
@@ -994,7 +1006,7 @@
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B24" s="10">
         <f t="shared" si="2"/>
@@ -1012,7 +1024,7 @@
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B25" s="10">
         <f t="shared" si="2"/>
@@ -1030,7 +1042,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B26" s="10">
         <f t="shared" si="2"/>
@@ -1048,7 +1060,7 @@
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B27" s="10">
         <f t="shared" si="2"/>
@@ -1066,7 +1078,7 @@
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B28" s="10">
         <f t="shared" si="2"/>
@@ -1084,7 +1096,7 @@
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B29" s="10">
         <f t="shared" si="2"/>
@@ -1102,7 +1114,7 @@
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B30" s="11">
         <f t="shared" si="2"/>
@@ -1120,7 +1132,7 @@
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B31" s="10">
         <f t="shared" si="2"/>
@@ -1138,7 +1150,7 @@
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B32" s="10">
         <f t="shared" si="2"/>
@@ -1156,7 +1168,7 @@
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B33" s="10">
         <f t="shared" si="2"/>
@@ -1174,7 +1186,7 @@
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B34" s="10">
         <f t="shared" si="2"/>
@@ -1192,7 +1204,7 @@
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B35" s="10">
         <f t="shared" si="2"/>
@@ -1210,7 +1222,7 @@
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B36" s="10">
         <f t="shared" si="2"/>
@@ -1228,7 +1240,7 @@
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B37" s="10">
         <f t="shared" si="2"/>
@@ -1246,7 +1258,7 @@
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B38" s="10">
         <f t="shared" si="2"/>
@@ -1264,7 +1276,7 @@
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B39" s="10">
         <f t="shared" si="2"/>
@@ -1282,7 +1294,7 @@
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B40" s="10">
         <f t="shared" si="2"/>
@@ -1300,7 +1312,7 @@
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B41" s="10">
         <f t="shared" si="2"/>
@@ -1318,7 +1330,7 @@
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B42" s="10">
         <f t="shared" si="2"/>
@@ -1336,7 +1348,7 @@
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B43" s="10">
         <f t="shared" si="2"/>
@@ -1354,7 +1366,7 @@
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B44" s="10">
         <f t="shared" si="2"/>
@@ -1372,7 +1384,7 @@
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B45" s="10">
         <f t="shared" si="2"/>
@@ -1390,7 +1402,7 @@
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="str">
         <f t="shared" ref="A46:A109" si="4">A45</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B46" s="11">
         <f t="shared" si="2"/>
@@ -1408,7 +1420,7 @@
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B47" s="10">
         <f t="shared" si="2"/>
@@ -1426,7 +1438,7 @@
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B48" s="10">
         <f t="shared" si="2"/>
@@ -1444,7 +1456,7 @@
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B49" s="10">
         <f t="shared" si="2"/>
@@ -1462,7 +1474,7 @@
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B50" s="10">
         <f t="shared" si="2"/>
@@ -1480,7 +1492,7 @@
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B51" s="10">
         <f t="shared" si="2"/>
@@ -1498,7 +1510,7 @@
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B52" s="10">
         <f t="shared" si="2"/>
@@ -1516,7 +1528,7 @@
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B53" s="10">
         <f t="shared" si="2"/>
@@ -1534,7 +1546,7 @@
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B54" s="10">
         <f t="shared" ref="B54:B117" si="5">C53</f>
@@ -1552,7 +1564,7 @@
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B55" s="10">
         <f t="shared" si="5"/>
@@ -1570,7 +1582,7 @@
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B56" s="10">
         <f t="shared" si="5"/>
@@ -1588,7 +1600,7 @@
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B57" s="10">
         <f t="shared" si="5"/>
@@ -1606,7 +1618,7 @@
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B58" s="10">
         <f t="shared" si="5"/>
@@ -1624,7 +1636,7 @@
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B59" s="10">
         <f t="shared" si="5"/>
@@ -1642,7 +1654,7 @@
     <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B60" s="10">
         <f t="shared" si="5"/>
@@ -1660,7 +1672,7 @@
     <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B61" s="10">
         <f t="shared" si="5"/>
@@ -1678,7 +1690,7 @@
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B62" s="11">
         <f t="shared" si="5"/>
@@ -1696,7 +1708,7 @@
     <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B63" s="10">
         <f t="shared" si="5"/>
@@ -1714,7 +1726,7 @@
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B64" s="10">
         <f t="shared" si="5"/>
@@ -1732,7 +1744,7 @@
     <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B65" s="10">
         <f t="shared" si="5"/>
@@ -1750,7 +1762,7 @@
     <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B66" s="10">
         <f t="shared" si="5"/>
@@ -1768,7 +1780,7 @@
     <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B67" s="10">
         <f t="shared" si="5"/>
@@ -1786,7 +1798,7 @@
     <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B68" s="10">
         <f t="shared" si="5"/>
@@ -1804,7 +1816,7 @@
     <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B69" s="10">
         <f t="shared" si="5"/>
@@ -1822,7 +1834,7 @@
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B70" s="10">
         <f t="shared" si="5"/>
@@ -1840,7 +1852,7 @@
     <row r="71" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B71" s="10">
         <f t="shared" si="5"/>
@@ -1858,7 +1870,7 @@
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B72" s="10">
         <f t="shared" si="5"/>
@@ -1876,7 +1888,7 @@
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B73" s="10">
         <f t="shared" si="5"/>
@@ -1894,7 +1906,7 @@
     <row r="74" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B74" s="10">
         <f t="shared" si="5"/>
@@ -1912,7 +1924,7 @@
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B75" s="10">
         <f t="shared" si="5"/>
@@ -1930,7 +1942,7 @@
     <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B76" s="10">
         <f t="shared" si="5"/>
@@ -1948,7 +1960,7 @@
     <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B77" s="10">
         <f t="shared" si="5"/>
@@ -1966,7 +1978,7 @@
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B78" s="11">
         <f t="shared" si="5"/>
@@ -1984,7 +1996,7 @@
     <row r="79" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B79" s="10">
         <f t="shared" si="5"/>
@@ -2002,7 +2014,7 @@
     <row r="80" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B80" s="10">
         <f t="shared" si="5"/>
@@ -2020,7 +2032,7 @@
     <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B81" s="10">
         <f t="shared" si="5"/>
@@ -2038,7 +2050,7 @@
     <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B82" s="10">
         <f t="shared" si="5"/>
@@ -2056,7 +2068,7 @@
     <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B83" s="10">
         <f t="shared" si="5"/>
@@ -2074,7 +2086,7 @@
     <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B84" s="10">
         <f t="shared" si="5"/>
@@ -2092,7 +2104,7 @@
     <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B85" s="10">
         <f t="shared" si="5"/>
@@ -2110,7 +2122,7 @@
     <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B86" s="10">
         <f t="shared" si="5"/>
@@ -2128,7 +2140,7 @@
     <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B87" s="10">
         <f t="shared" si="5"/>
@@ -2146,7 +2158,7 @@
     <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B88" s="10">
         <f t="shared" si="5"/>
@@ -2164,7 +2176,7 @@
     <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B89" s="10">
         <f t="shared" si="5"/>
@@ -2182,7 +2194,7 @@
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B90" s="10">
         <f t="shared" si="5"/>
@@ -2200,7 +2212,7 @@
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B91" s="10">
         <f t="shared" si="5"/>
@@ -2218,7 +2230,7 @@
     <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B92" s="10">
         <f t="shared" si="5"/>
@@ -2236,7 +2248,7 @@
     <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B93" s="10">
         <f t="shared" si="5"/>
@@ -2254,7 +2266,7 @@
     <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B94" s="11">
         <f t="shared" si="5"/>
@@ -2272,7 +2284,7 @@
     <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B95" s="10">
         <f t="shared" si="5"/>
@@ -2290,7 +2302,7 @@
     <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B96" s="10">
         <f t="shared" si="5"/>
@@ -2308,7 +2320,7 @@
     <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B97" s="10">
         <f t="shared" si="5"/>
@@ -2326,7 +2338,7 @@
     <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B98" s="10">
         <f t="shared" si="5"/>
@@ -2344,7 +2356,7 @@
     <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B99" s="10">
         <f t="shared" si="5"/>
@@ -2362,7 +2374,7 @@
     <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B100" s="10">
         <f t="shared" si="5"/>
@@ -2380,7 +2392,7 @@
     <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B101" s="10">
         <f t="shared" si="5"/>
@@ -2398,7 +2410,7 @@
     <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B102" s="10">
         <f t="shared" si="5"/>
@@ -2416,7 +2428,7 @@
     <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B103" s="10">
         <f t="shared" si="5"/>
@@ -2434,7 +2446,7 @@
     <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B104" s="10">
         <f t="shared" si="5"/>
@@ -2452,7 +2464,7 @@
     <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B105" s="10">
         <f t="shared" si="5"/>
@@ -2470,7 +2482,7 @@
     <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B106" s="10">
         <f t="shared" si="5"/>
@@ -2488,7 +2500,7 @@
     <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B107" s="10">
         <f t="shared" si="5"/>
@@ -2506,7 +2518,7 @@
     <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B108" s="10">
         <f t="shared" si="5"/>
@@ -2524,7 +2536,7 @@
     <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B109" s="10">
         <f t="shared" si="5"/>
@@ -2542,7 +2554,7 @@
     <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="str">
         <f t="shared" ref="A110:A173" si="7">A109</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B110" s="11">
         <f t="shared" si="5"/>
@@ -2560,7 +2572,7 @@
     <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B111" s="10">
         <f t="shared" si="5"/>
@@ -2578,7 +2590,7 @@
     <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B112" s="10">
         <f t="shared" si="5"/>
@@ -2596,7 +2608,7 @@
     <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B113" s="10">
         <f t="shared" si="5"/>
@@ -2614,7 +2626,7 @@
     <row r="114" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B114" s="10">
         <f t="shared" si="5"/>
@@ -2632,7 +2644,7 @@
     <row r="115" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B115" s="10">
         <f t="shared" si="5"/>
@@ -2650,7 +2662,7 @@
     <row r="116" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B116" s="10">
         <f t="shared" si="5"/>
@@ -2668,7 +2680,7 @@
     <row r="117" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B117" s="10">
         <f t="shared" si="5"/>
@@ -2686,7 +2698,7 @@
     <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B118" s="10">
         <f t="shared" ref="B118:B181" si="8">C117</f>
@@ -2704,7 +2716,7 @@
     <row r="119" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B119" s="10">
         <f t="shared" si="8"/>
@@ -2722,7 +2734,7 @@
     <row r="120" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B120" s="10">
         <f t="shared" si="8"/>
@@ -2740,7 +2752,7 @@
     <row r="121" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B121" s="10">
         <f t="shared" si="8"/>
@@ -2758,7 +2770,7 @@
     <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B122" s="10">
         <f t="shared" si="8"/>
@@ -2776,7 +2788,7 @@
     <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B123" s="10">
         <f t="shared" si="8"/>
@@ -2794,7 +2806,7 @@
     <row r="124" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B124" s="10">
         <f t="shared" si="8"/>
@@ -2812,7 +2824,7 @@
     <row r="125" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B125" s="10">
         <f t="shared" si="8"/>
@@ -2830,7 +2842,7 @@
     <row r="126" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B126" s="11">
         <f t="shared" si="8"/>
@@ -2848,7 +2860,7 @@
     <row r="127" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B127" s="10">
         <f t="shared" si="8"/>
@@ -2866,7 +2878,7 @@
     <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B128" s="10">
         <f t="shared" si="8"/>
@@ -2884,7 +2896,7 @@
     <row r="129" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B129" s="10">
         <f t="shared" si="8"/>
@@ -2902,7 +2914,7 @@
     <row r="130" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B130" s="10">
         <f t="shared" si="8"/>
@@ -2920,7 +2932,7 @@
     <row r="131" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B131" s="10">
         <f t="shared" si="8"/>
@@ -2938,7 +2950,7 @@
     <row r="132" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B132" s="10">
         <f t="shared" si="8"/>
@@ -2956,7 +2968,7 @@
     <row r="133" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B133" s="10">
         <f t="shared" si="8"/>
@@ -2974,7 +2986,7 @@
     <row r="134" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B134" s="10">
         <f t="shared" si="8"/>
@@ -2992,7 +3004,7 @@
     <row r="135" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B135" s="10">
         <f t="shared" si="8"/>
@@ -3010,7 +3022,7 @@
     <row r="136" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B136" s="10">
         <f t="shared" si="8"/>
@@ -3028,7 +3040,7 @@
     <row r="137" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B137" s="10">
         <f t="shared" si="8"/>
@@ -3046,7 +3058,7 @@
     <row r="138" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B138" s="10">
         <f t="shared" si="8"/>
@@ -3064,7 +3076,7 @@
     <row r="139" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B139" s="10">
         <f t="shared" si="8"/>
@@ -3082,7 +3094,7 @@
     <row r="140" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B140" s="10">
         <f t="shared" si="8"/>
@@ -3100,7 +3112,7 @@
     <row r="141" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B141" s="10">
         <f t="shared" si="8"/>
@@ -3118,7 +3130,7 @@
     <row r="142" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B142" s="11">
         <f t="shared" si="8"/>
@@ -3136,7 +3148,7 @@
     <row r="143" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B143" s="10">
         <f t="shared" si="8"/>
@@ -3154,7 +3166,7 @@
     <row r="144" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B144" s="10">
         <f t="shared" si="8"/>
@@ -3172,7 +3184,7 @@
     <row r="145" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B145" s="10">
         <f t="shared" si="8"/>
@@ -3190,7 +3202,7 @@
     <row r="146" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B146" s="10">
         <f t="shared" si="8"/>
@@ -3208,7 +3220,7 @@
     <row r="147" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B147" s="10">
         <f t="shared" si="8"/>
@@ -3226,7 +3238,7 @@
     <row r="148" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B148" s="10">
         <f t="shared" si="8"/>
@@ -3244,7 +3256,7 @@
     <row r="149" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B149" s="10">
         <f t="shared" si="8"/>
@@ -3262,7 +3274,7 @@
     <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B150" s="10">
         <f t="shared" si="8"/>
@@ -3280,7 +3292,7 @@
     <row r="151" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B151" s="10">
         <f t="shared" si="8"/>
@@ -3298,7 +3310,7 @@
     <row r="152" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B152" s="10">
         <f t="shared" si="8"/>
@@ -3316,7 +3328,7 @@
     <row r="153" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B153" s="10">
         <f t="shared" si="8"/>
@@ -3334,7 +3346,7 @@
     <row r="154" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B154" s="10">
         <f t="shared" si="8"/>
@@ -3352,7 +3364,7 @@
     <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B155" s="10">
         <f t="shared" si="8"/>
@@ -3370,7 +3382,7 @@
     <row r="156" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B156" s="10">
         <f t="shared" si="8"/>
@@ -3388,7 +3400,7 @@
     <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B157" s="10">
         <f t="shared" si="8"/>
@@ -3406,7 +3418,7 @@
     <row r="158" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B158" s="11">
         <f t="shared" si="8"/>
@@ -3424,7 +3436,7 @@
     <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B159" s="10">
         <f t="shared" si="8"/>
@@ -3442,7 +3454,7 @@
     <row r="160" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B160" s="10">
         <f t="shared" si="8"/>
@@ -3460,7 +3472,7 @@
     <row r="161" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B161" s="10">
         <f t="shared" si="8"/>
@@ -3478,7 +3490,7 @@
     <row r="162" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B162" s="10">
         <f t="shared" si="8"/>
@@ -3496,7 +3508,7 @@
     <row r="163" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B163" s="10">
         <f t="shared" si="8"/>
@@ -3514,7 +3526,7 @@
     <row r="164" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B164" s="10">
         <f t="shared" si="8"/>
@@ -3532,7 +3544,7 @@
     <row r="165" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B165" s="10">
         <f t="shared" si="8"/>
@@ -3550,7 +3562,7 @@
     <row r="166" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B166" s="10">
         <f t="shared" si="8"/>
@@ -3568,7 +3580,7 @@
     <row r="167" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B167" s="10">
         <f t="shared" si="8"/>
@@ -3586,7 +3598,7 @@
     <row r="168" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B168" s="10">
         <f t="shared" si="8"/>
@@ -3604,7 +3616,7 @@
     <row r="169" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B169" s="10">
         <f t="shared" si="8"/>
@@ -3622,7 +3634,7 @@
     <row r="170" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B170" s="10">
         <f t="shared" si="8"/>
@@ -3640,7 +3652,7 @@
     <row r="171" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B171" s="10">
         <f t="shared" si="8"/>
@@ -3658,7 +3670,7 @@
     <row r="172" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="8" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B172" s="10">
         <f t="shared" si="8"/>
@@ -3676,7 +3688,7 @@
     <row r="173" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B173" s="10">
         <f t="shared" si="8"/>
@@ -3694,7 +3706,7 @@
     <row r="174" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="8" t="str">
         <f t="shared" ref="A174:A237" si="10">A173</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B174" s="11">
         <f t="shared" si="8"/>
@@ -3712,7 +3724,7 @@
     <row r="175" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B175" s="10">
         <f t="shared" si="8"/>
@@ -3730,7 +3742,7 @@
     <row r="176" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B176" s="10">
         <f t="shared" si="8"/>
@@ -3748,7 +3760,7 @@
     <row r="177" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B177" s="10">
         <f t="shared" si="8"/>
@@ -3766,7 +3778,7 @@
     <row r="178" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B178" s="10">
         <f t="shared" si="8"/>
@@ -3784,7 +3796,7 @@
     <row r="179" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B179" s="10">
         <f t="shared" si="8"/>
@@ -3802,7 +3814,7 @@
     <row r="180" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B180" s="10">
         <f t="shared" si="8"/>
@@ -3820,7 +3832,7 @@
     <row r="181" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B181" s="10">
         <f t="shared" si="8"/>
@@ -3838,7 +3850,7 @@
     <row r="182" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B182" s="10">
         <f t="shared" ref="B182:B245" si="11">C181</f>
@@ -3856,7 +3868,7 @@
     <row r="183" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B183" s="10">
         <f t="shared" si="11"/>
@@ -3874,7 +3886,7 @@
     <row r="184" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B184" s="10">
         <f t="shared" si="11"/>
@@ -3892,7 +3904,7 @@
     <row r="185" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B185" s="10">
         <f t="shared" si="11"/>
@@ -3910,7 +3922,7 @@
     <row r="186" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B186" s="10">
         <f t="shared" si="11"/>
@@ -3928,7 +3940,7 @@
     <row r="187" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B187" s="10">
         <f t="shared" si="11"/>
@@ -3946,7 +3958,7 @@
     <row r="188" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B188" s="10">
         <f t="shared" si="11"/>
@@ -3964,7 +3976,7 @@
     <row r="189" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B189" s="10">
         <f t="shared" si="11"/>
@@ -3982,7 +3994,7 @@
     <row r="190" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B190" s="11">
         <f t="shared" si="11"/>
@@ -4000,7 +4012,7 @@
     <row r="191" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B191" s="10">
         <f t="shared" si="11"/>
@@ -4018,7 +4030,7 @@
     <row r="192" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B192" s="10">
         <f t="shared" si="11"/>
@@ -4036,7 +4048,7 @@
     <row r="193" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B193" s="10">
         <f t="shared" si="11"/>
@@ -4054,7 +4066,7 @@
     <row r="194" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B194" s="10">
         <f t="shared" si="11"/>
@@ -4072,7 +4084,7 @@
     <row r="195" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B195" s="10">
         <f t="shared" si="11"/>
@@ -4090,7 +4102,7 @@
     <row r="196" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B196" s="10">
         <f t="shared" si="11"/>
@@ -4108,7 +4120,7 @@
     <row r="197" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B197" s="10">
         <f t="shared" si="11"/>
@@ -4126,7 +4138,7 @@
     <row r="198" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B198" s="10">
         <f t="shared" si="11"/>
@@ -4144,7 +4156,7 @@
     <row r="199" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B199" s="10">
         <f t="shared" si="11"/>
@@ -4162,7 +4174,7 @@
     <row r="200" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B200" s="10">
         <f t="shared" si="11"/>
@@ -4180,7 +4192,7 @@
     <row r="201" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B201" s="10">
         <f t="shared" si="11"/>
@@ -4198,7 +4210,7 @@
     <row r="202" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B202" s="10">
         <f t="shared" si="11"/>
@@ -4216,7 +4228,7 @@
     <row r="203" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B203" s="10">
         <f t="shared" si="11"/>
@@ -4234,7 +4246,7 @@
     <row r="204" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B204" s="10">
         <f t="shared" si="11"/>
@@ -4252,7 +4264,7 @@
     <row r="205" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B205" s="10">
         <f t="shared" si="11"/>
@@ -4270,7 +4282,7 @@
     <row r="206" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B206" s="11">
         <f t="shared" si="11"/>
@@ -4288,7 +4300,7 @@
     <row r="207" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B207" s="10">
         <f t="shared" si="11"/>
@@ -4306,7 +4318,7 @@
     <row r="208" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B208" s="10">
         <f t="shared" si="11"/>
@@ -4324,7 +4336,7 @@
     <row r="209" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B209" s="10">
         <f t="shared" si="11"/>
@@ -4342,7 +4354,7 @@
     <row r="210" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B210" s="10">
         <f t="shared" si="11"/>
@@ -4360,7 +4372,7 @@
     <row r="211" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B211" s="10">
         <f t="shared" si="11"/>
@@ -4378,7 +4390,7 @@
     <row r="212" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B212" s="10">
         <f t="shared" si="11"/>
@@ -4396,7 +4408,7 @@
     <row r="213" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B213" s="10">
         <f t="shared" si="11"/>
@@ -4414,7 +4426,7 @@
     <row r="214" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B214" s="10">
         <f t="shared" si="11"/>
@@ -4432,7 +4444,7 @@
     <row r="215" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B215" s="10">
         <f t="shared" si="11"/>
@@ -4450,7 +4462,7 @@
     <row r="216" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B216" s="10">
         <f t="shared" si="11"/>
@@ -4468,7 +4480,7 @@
     <row r="217" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B217" s="10">
         <f t="shared" si="11"/>
@@ -4486,7 +4498,7 @@
     <row r="218" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B218" s="10">
         <f t="shared" si="11"/>
@@ -4504,7 +4516,7 @@
     <row r="219" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B219" s="10">
         <f t="shared" si="11"/>
@@ -4522,7 +4534,7 @@
     <row r="220" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B220" s="10">
         <f t="shared" si="11"/>
@@ -4540,7 +4552,7 @@
     <row r="221" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B221" s="10">
         <f t="shared" si="11"/>
@@ -4558,7 +4570,7 @@
     <row r="222" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B222" s="11">
         <f t="shared" si="11"/>
@@ -4576,7 +4588,7 @@
     <row r="223" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B223" s="10">
         <f t="shared" si="11"/>
@@ -4594,7 +4606,7 @@
     <row r="224" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B224" s="10">
         <f t="shared" si="11"/>
@@ -4612,7 +4624,7 @@
     <row r="225" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B225" s="10">
         <f t="shared" si="11"/>
@@ -4630,7 +4642,7 @@
     <row r="226" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B226" s="10">
         <f t="shared" si="11"/>
@@ -4648,7 +4660,7 @@
     <row r="227" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B227" s="10">
         <f t="shared" si="11"/>
@@ -4666,7 +4678,7 @@
     <row r="228" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B228" s="10">
         <f t="shared" si="11"/>
@@ -4684,7 +4696,7 @@
     <row r="229" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B229" s="10">
         <f t="shared" si="11"/>
@@ -4702,7 +4714,7 @@
     <row r="230" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B230" s="10">
         <f t="shared" si="11"/>
@@ -4720,7 +4732,7 @@
     <row r="231" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B231" s="10">
         <f t="shared" si="11"/>
@@ -4738,7 +4750,7 @@
     <row r="232" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B232" s="10">
         <f t="shared" si="11"/>
@@ -4756,7 +4768,7 @@
     <row r="233" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B233" s="10">
         <f t="shared" si="11"/>
@@ -4774,7 +4786,7 @@
     <row r="234" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B234" s="10">
         <f t="shared" si="11"/>
@@ -4792,7 +4804,7 @@
     <row r="235" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B235" s="10">
         <f t="shared" si="11"/>
@@ -4810,7 +4822,7 @@
     <row r="236" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="8" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B236" s="10">
         <f t="shared" si="11"/>
@@ -4828,7 +4840,7 @@
     <row r="237" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B237" s="10">
         <f t="shared" si="11"/>
@@ -4846,7 +4858,7 @@
     <row r="238" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="8" t="str">
         <f t="shared" ref="A238:A301" si="13">A237</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B238" s="11">
         <f t="shared" si="11"/>
@@ -4864,7 +4876,7 @@
     <row r="239" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B239" s="10">
         <f t="shared" si="11"/>
@@ -4882,7 +4894,7 @@
     <row r="240" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B240" s="10">
         <f t="shared" si="11"/>
@@ -4900,7 +4912,7 @@
     <row r="241" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B241" s="10">
         <f t="shared" si="11"/>
@@ -4918,7 +4930,7 @@
     <row r="242" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B242" s="10">
         <f t="shared" si="11"/>
@@ -4936,7 +4948,7 @@
     <row r="243" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B243" s="10">
         <f t="shared" si="11"/>
@@ -4954,7 +4966,7 @@
     <row r="244" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B244" s="10">
         <f t="shared" si="11"/>
@@ -4972,7 +4984,7 @@
     <row r="245" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B245" s="10">
         <f t="shared" si="11"/>
@@ -4990,7 +5002,7 @@
     <row r="246" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B246" s="10">
         <f t="shared" ref="B246:B309" si="14">C245</f>
@@ -5008,7 +5020,7 @@
     <row r="247" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B247" s="10">
         <f t="shared" si="14"/>
@@ -5026,7 +5038,7 @@
     <row r="248" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B248" s="10">
         <f t="shared" si="14"/>
@@ -5044,7 +5056,7 @@
     <row r="249" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B249" s="10">
         <f t="shared" si="14"/>
@@ -5062,7 +5074,7 @@
     <row r="250" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B250" s="10">
         <f t="shared" si="14"/>
@@ -5080,7 +5092,7 @@
     <row r="251" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B251" s="10">
         <f t="shared" si="14"/>
@@ -5098,7 +5110,7 @@
     <row r="252" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B252" s="10">
         <f t="shared" si="14"/>
@@ -5116,7 +5128,7 @@
     <row r="253" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B253" s="10">
         <f t="shared" si="14"/>
@@ -5134,7 +5146,7 @@
     <row r="254" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B254" s="11">
         <f t="shared" si="14"/>
@@ -5152,7 +5164,7 @@
     <row r="255" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B255" s="10">
         <f t="shared" si="14"/>
@@ -5170,7 +5182,7 @@
     <row r="256" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B256" s="10">
         <f t="shared" si="14"/>
@@ -5188,7 +5200,7 @@
     <row r="257" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B257" s="10">
         <f t="shared" si="14"/>
@@ -5206,7 +5218,7 @@
     <row r="258" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B258" s="10">
         <f t="shared" si="14"/>
@@ -5224,7 +5236,7 @@
     <row r="259" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B259" s="10">
         <f t="shared" si="14"/>
@@ -5242,7 +5254,7 @@
     <row r="260" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B260" s="10">
         <f t="shared" si="14"/>
@@ -5260,7 +5272,7 @@
     <row r="261" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B261" s="10">
         <f t="shared" si="14"/>
@@ -5278,7 +5290,7 @@
     <row r="262" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B262" s="10">
         <f t="shared" si="14"/>
@@ -5296,7 +5308,7 @@
     <row r="263" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B263" s="10">
         <f t="shared" si="14"/>
@@ -5314,7 +5326,7 @@
     <row r="264" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B264" s="10">
         <f t="shared" si="14"/>
@@ -5332,7 +5344,7 @@
     <row r="265" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B265" s="10">
         <f t="shared" si="14"/>
@@ -5350,7 +5362,7 @@
     <row r="266" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B266" s="10">
         <f t="shared" si="14"/>
@@ -5368,7 +5380,7 @@
     <row r="267" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B267" s="10">
         <f t="shared" si="14"/>
@@ -5386,7 +5398,7 @@
     <row r="268" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B268" s="10">
         <f t="shared" si="14"/>
@@ -5404,7 +5416,7 @@
     <row r="269" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B269" s="10">
         <f t="shared" si="14"/>
@@ -5422,7 +5434,7 @@
     <row r="270" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B270" s="11">
         <f t="shared" si="14"/>
@@ -5440,7 +5452,7 @@
     <row r="271" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B271" s="10">
         <f t="shared" si="14"/>
@@ -5458,7 +5470,7 @@
     <row r="272" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B272" s="10">
         <f t="shared" si="14"/>
@@ -5476,7 +5488,7 @@
     <row r="273" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B273" s="10">
         <f t="shared" si="14"/>
@@ -5494,7 +5506,7 @@
     <row r="274" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B274" s="10">
         <f t="shared" si="14"/>
@@ -5512,7 +5524,7 @@
     <row r="275" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B275" s="10">
         <f t="shared" si="14"/>
@@ -5530,7 +5542,7 @@
     <row r="276" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B276" s="10">
         <f t="shared" si="14"/>
@@ -5548,7 +5560,7 @@
     <row r="277" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B277" s="10">
         <f t="shared" si="14"/>
@@ -5566,7 +5578,7 @@
     <row r="278" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B278" s="10">
         <f t="shared" si="14"/>
@@ -5584,7 +5596,7 @@
     <row r="279" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B279" s="10">
         <f t="shared" si="14"/>
@@ -5602,7 +5614,7 @@
     <row r="280" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B280" s="10">
         <f t="shared" si="14"/>
@@ -5620,7 +5632,7 @@
     <row r="281" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B281" s="10">
         <f t="shared" si="14"/>
@@ -5638,7 +5650,7 @@
     <row r="282" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B282" s="10">
         <f t="shared" si="14"/>
@@ -5656,7 +5668,7 @@
     <row r="283" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B283" s="10">
         <f t="shared" si="14"/>
@@ -5674,7 +5686,7 @@
     <row r="284" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B284" s="10">
         <f t="shared" si="14"/>
@@ -5692,7 +5704,7 @@
     <row r="285" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B285" s="10">
         <f t="shared" si="14"/>
@@ -5710,7 +5722,7 @@
     <row r="286" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B286" s="11">
         <f t="shared" si="14"/>
@@ -5728,7 +5740,7 @@
     <row r="287" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B287" s="10">
         <f t="shared" si="14"/>
@@ -5746,7 +5758,7 @@
     <row r="288" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B288" s="10">
         <f t="shared" si="14"/>
@@ -5764,7 +5776,7 @@
     <row r="289" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B289" s="10">
         <f t="shared" si="14"/>
@@ -5782,7 +5794,7 @@
     <row r="290" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B290" s="10">
         <f t="shared" si="14"/>
@@ -5800,7 +5812,7 @@
     <row r="291" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B291" s="10">
         <f t="shared" si="14"/>
@@ -5818,7 +5830,7 @@
     <row r="292" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B292" s="10">
         <f t="shared" si="14"/>
@@ -5836,7 +5848,7 @@
     <row r="293" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B293" s="10">
         <f t="shared" si="14"/>
@@ -5854,7 +5866,7 @@
     <row r="294" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B294" s="10">
         <f t="shared" si="14"/>
@@ -5872,7 +5884,7 @@
     <row r="295" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B295" s="10">
         <f t="shared" si="14"/>
@@ -5890,7 +5902,7 @@
     <row r="296" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B296" s="10">
         <f t="shared" si="14"/>
@@ -5908,7 +5920,7 @@
     <row r="297" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B297" s="10">
         <f t="shared" si="14"/>
@@ -5926,7 +5938,7 @@
     <row r="298" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B298" s="10">
         <f t="shared" si="14"/>
@@ -5944,7 +5956,7 @@
     <row r="299" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B299" s="10">
         <f t="shared" si="14"/>
@@ -5962,7 +5974,7 @@
     <row r="300" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="8" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B300" s="10">
         <f t="shared" si="14"/>
@@ -5980,7 +5992,7 @@
     <row r="301" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="7" t="str">
         <f t="shared" si="13"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B301" s="10">
         <f t="shared" si="14"/>
@@ -5998,7 +6010,7 @@
     <row r="302" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="8" t="str">
         <f t="shared" ref="A302:A365" si="16">A301</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B302" s="11">
         <f t="shared" si="14"/>
@@ -6016,7 +6028,7 @@
     <row r="303" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B303" s="10">
         <f t="shared" si="14"/>
@@ -6034,7 +6046,7 @@
     <row r="304" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B304" s="10">
         <f t="shared" si="14"/>
@@ -6052,7 +6064,7 @@
     <row r="305" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B305" s="10">
         <f t="shared" si="14"/>
@@ -6070,7 +6082,7 @@
     <row r="306" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B306" s="10">
         <f t="shared" si="14"/>
@@ -6088,7 +6100,7 @@
     <row r="307" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B307" s="10">
         <f t="shared" si="14"/>
@@ -6106,7 +6118,7 @@
     <row r="308" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B308" s="10">
         <f t="shared" si="14"/>
@@ -6124,7 +6136,7 @@
     <row r="309" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B309" s="10">
         <f t="shared" si="14"/>
@@ -6142,7 +6154,7 @@
     <row r="310" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B310" s="10">
         <f t="shared" ref="B310:B373" si="17">C309</f>
@@ -6160,7 +6172,7 @@
     <row r="311" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B311" s="10">
         <f t="shared" si="17"/>
@@ -6178,7 +6190,7 @@
     <row r="312" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B312" s="10">
         <f t="shared" si="17"/>
@@ -6196,7 +6208,7 @@
     <row r="313" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B313" s="10">
         <f t="shared" si="17"/>
@@ -6214,7 +6226,7 @@
     <row r="314" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B314" s="10">
         <f t="shared" si="17"/>
@@ -6232,7 +6244,7 @@
     <row r="315" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B315" s="10">
         <f t="shared" si="17"/>
@@ -6250,7 +6262,7 @@
     <row r="316" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B316" s="10">
         <f t="shared" si="17"/>
@@ -6268,7 +6280,7 @@
     <row r="317" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B317" s="10">
         <f t="shared" si="17"/>
@@ -6286,7 +6298,7 @@
     <row r="318" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B318" s="11">
         <f t="shared" si="17"/>
@@ -6304,7 +6316,7 @@
     <row r="319" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B319" s="10">
         <f t="shared" si="17"/>
@@ -6322,7 +6334,7 @@
     <row r="320" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B320" s="10">
         <f t="shared" si="17"/>
@@ -6340,7 +6352,7 @@
     <row r="321" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B321" s="10">
         <f t="shared" si="17"/>
@@ -6358,7 +6370,7 @@
     <row r="322" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B322" s="10">
         <f t="shared" si="17"/>
@@ -6376,7 +6388,7 @@
     <row r="323" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B323" s="10">
         <f t="shared" si="17"/>
@@ -6394,7 +6406,7 @@
     <row r="324" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B324" s="10">
         <f t="shared" si="17"/>
@@ -6412,7 +6424,7 @@
     <row r="325" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B325" s="10">
         <f t="shared" si="17"/>
@@ -6430,7 +6442,7 @@
     <row r="326" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B326" s="10">
         <f t="shared" si="17"/>
@@ -6448,7 +6460,7 @@
     <row r="327" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B327" s="10">
         <f t="shared" si="17"/>
@@ -6466,7 +6478,7 @@
     <row r="328" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B328" s="10">
         <f t="shared" si="17"/>
@@ -6484,7 +6496,7 @@
     <row r="329" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B329" s="10">
         <f t="shared" si="17"/>
@@ -6502,7 +6514,7 @@
     <row r="330" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B330" s="10">
         <f t="shared" si="17"/>
@@ -6520,7 +6532,7 @@
     <row r="331" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B331" s="10">
         <f t="shared" si="17"/>
@@ -6538,7 +6550,7 @@
     <row r="332" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B332" s="10">
         <f t="shared" si="17"/>
@@ -6556,7 +6568,7 @@
     <row r="333" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B333" s="10">
         <f t="shared" si="17"/>
@@ -6574,7 +6586,7 @@
     <row r="334" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B334" s="11">
         <f t="shared" si="17"/>
@@ -6592,7 +6604,7 @@
     <row r="335" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B335" s="10">
         <f t="shared" si="17"/>
@@ -6610,7 +6622,7 @@
     <row r="336" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B336" s="10">
         <f t="shared" si="17"/>
@@ -6628,7 +6640,7 @@
     <row r="337" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B337" s="10">
         <f t="shared" si="17"/>
@@ -6646,7 +6658,7 @@
     <row r="338" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B338" s="10">
         <f t="shared" si="17"/>
@@ -6664,7 +6676,7 @@
     <row r="339" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B339" s="10">
         <f t="shared" si="17"/>
@@ -6682,7 +6694,7 @@
     <row r="340" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B340" s="10">
         <f t="shared" si="17"/>
@@ -6700,7 +6712,7 @@
     <row r="341" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B341" s="10">
         <f t="shared" si="17"/>
@@ -6718,7 +6730,7 @@
     <row r="342" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B342" s="10">
         <f t="shared" si="17"/>
@@ -6736,7 +6748,7 @@
     <row r="343" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B343" s="10">
         <f t="shared" si="17"/>
@@ -6754,7 +6766,7 @@
     <row r="344" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B344" s="10">
         <f t="shared" si="17"/>
@@ -6772,7 +6784,7 @@
     <row r="345" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B345" s="10">
         <f t="shared" si="17"/>
@@ -6790,7 +6802,7 @@
     <row r="346" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B346" s="10">
         <f t="shared" si="17"/>
@@ -6808,7 +6820,7 @@
     <row r="347" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B347" s="10">
         <f t="shared" si="17"/>
@@ -6826,7 +6838,7 @@
     <row r="348" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B348" s="10">
         <f t="shared" si="17"/>
@@ -6844,7 +6856,7 @@
     <row r="349" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B349" s="10">
         <f t="shared" si="17"/>
@@ -6862,7 +6874,7 @@
     <row r="350" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B350" s="11">
         <f t="shared" si="17"/>
@@ -6880,7 +6892,7 @@
     <row r="351" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B351" s="10">
         <f t="shared" si="17"/>
@@ -6898,7 +6910,7 @@
     <row r="352" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B352" s="10">
         <f t="shared" si="17"/>
@@ -6916,7 +6928,7 @@
     <row r="353" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B353" s="10">
         <f t="shared" si="17"/>
@@ -6934,7 +6946,7 @@
     <row r="354" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B354" s="10">
         <f t="shared" si="17"/>
@@ -6952,7 +6964,7 @@
     <row r="355" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B355" s="10">
         <f t="shared" si="17"/>
@@ -6970,7 +6982,7 @@
     <row r="356" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B356" s="10">
         <f t="shared" si="17"/>
@@ -6988,7 +7000,7 @@
     <row r="357" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A357" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B357" s="10">
         <f t="shared" si="17"/>
@@ -7006,7 +7018,7 @@
     <row r="358" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B358" s="10">
         <f t="shared" si="17"/>
@@ -7024,7 +7036,7 @@
     <row r="359" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B359" s="10">
         <f t="shared" si="17"/>
@@ -7042,7 +7054,7 @@
     <row r="360" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A360" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B360" s="10">
         <f t="shared" si="17"/>
@@ -7060,7 +7072,7 @@
     <row r="361" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B361" s="10">
         <f t="shared" si="17"/>
@@ -7078,7 +7090,7 @@
     <row r="362" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A362" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B362" s="10">
         <f t="shared" si="17"/>
@@ -7096,7 +7108,7 @@
     <row r="363" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A363" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B363" s="10">
         <f t="shared" si="17"/>
@@ -7114,7 +7126,7 @@
     <row r="364" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A364" s="8" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B364" s="10">
         <f t="shared" si="17"/>
@@ -7132,7 +7144,7 @@
     <row r="365" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A365" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B365" s="10">
         <f t="shared" si="17"/>
@@ -7150,7 +7162,7 @@
     <row r="366" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A366" s="8" t="str">
         <f t="shared" ref="A366:A381" si="19">A365</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B366" s="11">
         <f t="shared" si="17"/>
@@ -7168,7 +7180,7 @@
     <row r="367" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A367" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B367" s="10">
         <f t="shared" si="17"/>
@@ -7186,7 +7198,7 @@
     <row r="368" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A368" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B368" s="10">
         <f t="shared" si="17"/>
@@ -7204,7 +7216,7 @@
     <row r="369" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A369" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B369" s="10">
         <f t="shared" si="17"/>
@@ -7222,7 +7234,7 @@
     <row r="370" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A370" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B370" s="10">
         <f t="shared" si="17"/>
@@ -7240,7 +7252,7 @@
     <row r="371" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A371" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B371" s="10">
         <f t="shared" si="17"/>
@@ -7258,7 +7270,7 @@
     <row r="372" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A372" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B372" s="10">
         <f t="shared" si="17"/>
@@ -7276,7 +7288,7 @@
     <row r="373" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A373" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B373" s="10">
         <f t="shared" si="17"/>
@@ -7294,7 +7306,7 @@
     <row r="374" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A374" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B374" s="10">
         <f t="shared" ref="B374:B381" si="20">C373</f>
@@ -7312,7 +7324,7 @@
     <row r="375" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A375" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B375" s="10">
         <f t="shared" si="20"/>
@@ -7330,7 +7342,7 @@
     <row r="376" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A376" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B376" s="10">
         <f t="shared" si="20"/>
@@ -7348,7 +7360,7 @@
     <row r="377" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A377" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B377" s="10">
         <f t="shared" si="20"/>
@@ -7366,7 +7378,7 @@
     <row r="378" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A378" s="8" t="str">
         <f>A377</f>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B378" s="10">
         <f t="shared" si="20"/>
@@ -7384,7 +7396,7 @@
     <row r="379" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B379" s="10">
         <f t="shared" si="20"/>
@@ -7402,7 +7414,7 @@
     <row r="380" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A380" s="8" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B380" s="10">
         <f t="shared" si="20"/>
@@ -7420,7 +7432,7 @@
     <row r="381" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A381" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>2020 09 11</v>
+        <v>2020 09 24</v>
       </c>
       <c r="B381" s="10">
         <f t="shared" si="20"/>

</xml_diff>